<commit_message>
Corrected the testprotocol and created the pdf
</commit_message>
<xml_diff>
--- a/Documents/c4pe_TestProtocol.xlsx
+++ b/Documents/c4pe_TestProtocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franzi Grausenburger\repos\c4pe\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E333A40-D302-4385-A819-474B0943BF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848902EA-63B4-4533-954D-FA91DA4BFDC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>Owner can't delete place, but admin can</t>
   </si>
   <si>
-    <t>Selecting a place type doesn't chage it from 'cafe'</t>
-  </si>
-  <si>
     <t>Create place type</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Tester:</t>
+  </si>
+  <si>
+    <t>Selecting a place type doesn't change it from 'cafe'</t>
   </si>
 </sst>
 </file>
@@ -305,56 +305,56 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -434,15 +434,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
+      <xdr:colOff>160020</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>662940</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -470,7 +470,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7078980" y="137160"/>
+          <a:off x="7063740" y="53340"/>
           <a:ext cx="2072640" cy="1089660"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -487,15 +487,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>188594</xdr:colOff>
+      <xdr:colOff>746760</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -523,8 +523,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3922394" y="5562600"/>
-          <a:ext cx="2326006" cy="1272540"/>
+          <a:off x="4480560" y="5730240"/>
+          <a:ext cx="1735454" cy="1082040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,444 +849,444 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
     </row>
     <row r="5" spans="2:10" ht="3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="4">
+      <c r="D5" s="11">
         <v>44000</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="13"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-    </row>
-    <row r="8" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="5"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-    </row>
-    <row r="9" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="2:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="2:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4">
         <v>6</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="8">
-        <v>2</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="C15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="4">
         <v>7</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="8">
-        <v>3</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="C16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="4">
         <v>8</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="8">
-        <v>4</v>
-      </c>
-      <c r="C13" s="9" t="s">
+      <c r="C17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="4">
         <v>9</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9" t="s">
+      <c r="C18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="4">
+        <v>10</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="4">
+        <v>11</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="4">
+        <v>12</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="4">
+        <v>13</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="4">
+        <v>14</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="4">
+        <v>15</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="4">
+        <v>16</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="4">
+        <v>17</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="2:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="8">
-        <v>5</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="4">
+        <v>18</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="2:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="4">
+        <v>19</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="5">
+        <v>20</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="3">
+        <v>21</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="2:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="8">
-        <v>6</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="8">
-        <v>7</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="8">
-        <v>8</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="8">
-        <v>9</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="8">
-        <v>10</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="8">
-        <v>11</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="8">
-        <v>12</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-    </row>
-    <row r="22" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="8">
-        <v>13</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="8">
-        <v>14</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="8">
-        <v>15</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="8">
-        <v>16</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="8">
-        <v>17</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="8">
-        <v>18</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="8">
-        <v>19</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-    </row>
-    <row r="29" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="11">
-        <v>20</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="7">
-        <v>21</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="14"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="19"/>
     </row>
     <row r="40" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="2:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1303,17 +1303,28 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="D1:H2"/>
+    <mergeCell ref="D3:H4"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="D5:H6"/>
     <mergeCell ref="E7:H8"/>
     <mergeCell ref="D7:D8"/>
@@ -1330,28 +1341,17 @@
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="D1:H2"/>
-    <mergeCell ref="D3:H4"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G15:J15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{67AF34C1-68CD-4195-A6E0-43EAD2931A02}"/>

</xml_diff>